<commit_message>
version des fichier excel
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>entite-cd01</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>code technique</t>
+  </si>
+  <si>
+    <t>toto_12</t>
   </si>
 </sst>
 </file>
@@ -372,9 +375,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -436,6 +441,11 @@
         <v>9</v>
       </c>
     </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>